<commit_message>
修复IndexError: list index out of range
</commit_message>
<xml_diff>
--- a/测试结果.xlsx
+++ b/测试结果.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,39 +441,17 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>期望输出</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
           <t>Agent回答</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>是否正确</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>中国在哪里？</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>中国的首都是北京哦。北京不仅是中国的政治中心，也是文化和国际交流的重要城市。如果你有更多关于北京或其他地方的问题，随时告诉我，我很乐意帮你解答。😊</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>中国位于东亚，是世界上面积第三大、人口最多的国家。它的东部和南部濒临太平洋，北部与俄罗斯和蒙古接壤，西部与哈萨克斯坦、吉尔吉斯斯坦、塔吉克斯坦等国接壤，西南部与印度、尼泊尔、不丹等国接壤，东南部与越南、老挝、缅甸等国接壤。中国有着悠久的历史和丰富的文化，是一个充满魅力的国家。如果你有更多关于中国的问题，随时告诉我哦！</t>
-        </is>
-      </c>
-      <c r="D2" t="b">
-        <v>0</v>
-      </c>
+          <t>（示例）中国的首都在哪里？</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -481,19 +459,7 @@
           <t>（示例）中国的首都在哪里？</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>中国的首都是北京哦。北京不仅是中国的政治中心，也是文化和国际交流的重要城市。如果你有更多关于北京或其他地方的问题，随时告诉我，我很乐意帮你解答。😊</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>中国的首都是北京哦。北京不仅是中国的政治中心，也是文化和国际交流的重要枢纽。如果你有更多关于北京或其他地方的问题，随时告诉我，我很乐意帮你解答。😊</t>
-        </is>
-      </c>
-      <c r="D3" t="b">
-        <v>1</v>
-      </c>
+      <c r="B3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -501,19 +467,15 @@
           <t>（示例）中国的首都在哪里？</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>中国的首都是北京哦。北京不仅是中国的政治中心，也是文化和国际交流的重要城市。如果你有更多关于北京或其他地方的问题，随时告诉我，我很乐意帮你解答。😊</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>中国的首都是北京哦。北京不仅是中国的政治中心，也是文化和教育的重要枢纽。如果你有更多关于北京或者其他地方的问题，随时告诉我哦！😊</t>
-        </is>
-      </c>
-      <c r="D4" t="b">
-        <v>1</v>
-      </c>
+      <c r="B4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>（示例）中国的首都在哪里？</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>